<commit_message>
Balancing and addition of Weapons
</commit_message>
<xml_diff>
--- a/Story/Balancing.xlsx
+++ b/Story/Balancing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub-GitKraken\Death is not the End\death-is-not-the-end\Story\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CE2BE5-2C39-4121-B056-6A3C30310C90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E25418E-A915-4D12-82AC-9966B32B9D48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Player" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="118">
   <si>
     <t>Speed</t>
   </si>
@@ -95,27 +95,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>don‘t</t>
-  </si>
-  <si>
-    <t>even</t>
-  </si>
-  <si>
-    <t>know</t>
-  </si>
-  <si>
-    <t>the</t>
-  </si>
-  <si>
-    <t>params</t>
-  </si>
-  <si>
-    <t>yet</t>
-  </si>
-  <si>
     <t>Same</t>
   </si>
   <si>
@@ -153,13 +132,265 @@
   </si>
   <si>
     <t>Super high jump with damage up to 20</t>
+  </si>
+  <si>
+    <t>Weapon Name</t>
+  </si>
+  <si>
+    <t>Wooden Sword</t>
+  </si>
+  <si>
+    <t>Wooden Lance</t>
+  </si>
+  <si>
+    <t>Wooden Longsword</t>
+  </si>
+  <si>
+    <t>Wooden Bow</t>
+  </si>
+  <si>
+    <t>Wooden Dagger</t>
+  </si>
+  <si>
+    <t>Wooden Weapons</t>
+  </si>
+  <si>
+    <t>Stone Weapons</t>
+  </si>
+  <si>
+    <t>Stone Sword</t>
+  </si>
+  <si>
+    <t>Stone Longsword</t>
+  </si>
+  <si>
+    <t>Stone Dagger</t>
+  </si>
+  <si>
+    <t>Stone Lance</t>
+  </si>
+  <si>
+    <t>Stone Bow (not out of Stone empowered with Stone)</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Metal Weapons</t>
+  </si>
+  <si>
+    <t>Metal Sword</t>
+  </si>
+  <si>
+    <t>Metal Longsword</t>
+  </si>
+  <si>
+    <t>Metal Dagger</t>
+  </si>
+  <si>
+    <t>Metal Lance</t>
+  </si>
+  <si>
+    <t>Metal Bow (look above)</t>
+  </si>
+  <si>
+    <t>Rusty Weapons</t>
+  </si>
+  <si>
+    <t>Rusty Sword</t>
+  </si>
+  <si>
+    <t>Rusty Longsword</t>
+  </si>
+  <si>
+    <t>Rusty Dagger</t>
+  </si>
+  <si>
+    <t>Rusty Lance</t>
+  </si>
+  <si>
+    <t>Rusty Bow (look above)</t>
+  </si>
+  <si>
+    <t>Movement Speed (when carrying weapon)</t>
+  </si>
+  <si>
+    <t>Ability (special attack)</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>whirl attack</t>
+  </si>
+  <si>
+    <t>earthshatter</t>
+  </si>
+  <si>
+    <t>every three hits</t>
+  </si>
+  <si>
+    <t>every 15 secs</t>
+  </si>
+  <si>
+    <t>backstitch</t>
+  </si>
+  <si>
+    <t>double hit</t>
+  </si>
+  <si>
+    <t>arrows</t>
+  </si>
+  <si>
+    <t>no cooldown</t>
+  </si>
+  <si>
+    <t>other arrows cannot be used</t>
+  </si>
+  <si>
+    <t>Arrow</t>
+  </si>
+  <si>
+    <t>a hit in the back does double damage</t>
+  </si>
+  <si>
+    <t>triple hit</t>
+  </si>
+  <si>
+    <t>every 12 secs</t>
+  </si>
+  <si>
+    <t>every three hits or every 5 seconds</t>
+  </si>
+  <si>
+    <t>Wands</t>
+  </si>
+  <si>
+    <t>Magic Wand</t>
+  </si>
+  <si>
+    <t>Follow up</t>
+  </si>
+  <si>
+    <t>Projectile Speed</t>
+  </si>
+  <si>
+    <t>Wand</t>
+  </si>
+  <si>
+    <t>Burn</t>
+  </si>
+  <si>
+    <t>Type of Weapon</t>
+  </si>
+  <si>
+    <t>Melee</t>
+  </si>
+  <si>
+    <t>Long-/Shortranged</t>
+  </si>
+  <si>
+    <t>Target-Seeking</t>
+  </si>
+  <si>
+    <t>Jumpattack</t>
+  </si>
+  <si>
+    <t>Explanation Ability</t>
+  </si>
+  <si>
+    <t>a slash around the whole body</t>
+  </si>
+  <si>
+    <t>stun for 0,5 seconds</t>
+  </si>
+  <si>
+    <t>every fifth hit</t>
+  </si>
+  <si>
+    <t>pricks twice in the same time (Attack Speed)</t>
+  </si>
+  <si>
+    <t>Attack Speed (How many attacks in one second)</t>
+  </si>
+  <si>
+    <t>Damag (multiplier with Base Dmg)</t>
+  </si>
+  <si>
+    <t>Cooldwon Ability</t>
+  </si>
+  <si>
+    <t>Arrows have different effects and damage</t>
+  </si>
+  <si>
+    <t>every fifth hit pricks three times</t>
+  </si>
+  <si>
+    <t>attack Speed times 1,5 and three hits</t>
+  </si>
+  <si>
+    <t>Movement Speed decreased by 2000 (if not under 4000 already)</t>
+  </si>
+  <si>
+    <t>5 dps for two seconds</t>
+  </si>
+  <si>
+    <t>every 8 seconds</t>
+  </si>
+  <si>
+    <t>a jump over the enemy sticking the wand into its highest point</t>
+  </si>
+  <si>
+    <t>Melee Wand</t>
+  </si>
+  <si>
+    <t>Special Weapons</t>
+  </si>
+  <si>
+    <t>Trident</t>
+  </si>
+  <si>
+    <t>Scythe</t>
+  </si>
+  <si>
+    <t>Torch</t>
+  </si>
+  <si>
+    <t>Longranged Melee</t>
+  </si>
+  <si>
+    <t>Helper</t>
+  </si>
+  <si>
+    <t>Spawn a watermonster fighting on your side</t>
+  </si>
+  <si>
+    <t>when killing an enemy the 60 second cooldown resets</t>
+  </si>
+  <si>
+    <t>Spawn a undead creature</t>
+  </si>
+  <si>
+    <t>Arsonist</t>
+  </si>
+  <si>
+    <t>ignite an enemy with 10 dps for five seconds (takes 0,8 seconds)</t>
+  </si>
+  <si>
+    <t>Bumerang</t>
+  </si>
+  <si>
+    <t>Double-Trouble</t>
+  </si>
+  <si>
+    <t>its a bumerang…what do you think will happen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -175,6 +406,19 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -200,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify"/>
@@ -212,6 +456,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -528,7 +775,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -567,7 +814,7 @@
         <v>100</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +832,7 @@
   <dimension ref="B2:O5"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -608,16 +855,16 @@
         <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>7</v>
@@ -626,7 +873,7 @@
         <v>8</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>9</v>
@@ -672,10 +919,10 @@
         <v>10</v>
       </c>
       <c r="G4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I4" s="5" t="s">
         <v>14</v>
@@ -701,7 +948,7 @@
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C5">
         <v>25000</v>
@@ -716,19 +963,22 @@
         <v>50</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
         <v>15</v>
       </c>
       <c r="K5" t="s">
         <v>15</v>
+      </c>
+      <c r="L5">
+        <v>12</v>
       </c>
       <c r="M5" s="8" t="s">
         <v>16</v>
@@ -805,40 +1055,850 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>83</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>94</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="G1" t="s">
-        <v>27</v>
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>22000</v>
+      </c>
+      <c r="G5" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>0.8</v>
+      </c>
+      <c r="F6">
+        <v>18000</v>
+      </c>
+      <c r="G6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H6" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1.5</v>
+      </c>
+      <c r="F7">
+        <v>24000</v>
+      </c>
+      <c r="G7" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1.3</v>
+      </c>
+      <c r="F8">
+        <v>23000</v>
+      </c>
+      <c r="G8" t="s">
+        <v>62</v>
+      </c>
+      <c r="H8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" t="s">
+        <v>62</v>
+      </c>
+      <c r="J8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0.7</v>
+      </c>
+      <c r="F9">
+        <v>22000</v>
+      </c>
+      <c r="G9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" t="s">
+        <v>62</v>
+      </c>
+      <c r="I9" t="s">
+        <v>71</v>
+      </c>
+      <c r="J9">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>21000</v>
+      </c>
+      <c r="G12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H12" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>0.8</v>
+      </c>
+      <c r="F13">
+        <v>17000</v>
+      </c>
+      <c r="G13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I13" t="s">
+        <v>66</v>
+      </c>
+      <c r="J13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>1.5</v>
+      </c>
+      <c r="F14">
+        <v>23000</v>
+      </c>
+      <c r="G14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H14" t="s">
+        <v>73</v>
+      </c>
+      <c r="I14" t="s">
+        <v>62</v>
+      </c>
+      <c r="J14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>1.3</v>
+      </c>
+      <c r="F15">
+        <v>22000</v>
+      </c>
+      <c r="G15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>0.7</v>
+      </c>
+      <c r="F16">
+        <v>21000</v>
+      </c>
+      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="H16" t="s">
+        <v>96</v>
+      </c>
+      <c r="I16" t="s">
+        <v>70</v>
+      </c>
+      <c r="J16">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
+        <v>84</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>0.7</v>
+      </c>
+      <c r="F19">
+        <v>18000</v>
+      </c>
+      <c r="G19" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" t="s">
+        <v>62</v>
+      </c>
+      <c r="J19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D20">
+        <v>8</v>
+      </c>
+      <c r="E20">
+        <v>0.5</v>
+      </c>
+      <c r="F20">
+        <v>14000</v>
+      </c>
+      <c r="G20" t="s">
+        <v>62</v>
+      </c>
+      <c r="I20" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21">
+        <v>5</v>
+      </c>
+      <c r="E21">
+        <v>1.2</v>
+      </c>
+      <c r="F21">
+        <v>20000</v>
+      </c>
+      <c r="G21" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" t="s">
+        <v>62</v>
+      </c>
+      <c r="J21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>19000</v>
+      </c>
+      <c r="G22" t="s">
+        <v>62</v>
+      </c>
+      <c r="I22" t="s">
+        <v>62</v>
+      </c>
+      <c r="J22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23">
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <v>0.4</v>
+      </c>
+      <c r="F23">
+        <v>18000</v>
+      </c>
+      <c r="G23" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23" t="s">
+        <v>62</v>
+      </c>
+      <c r="J23">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>84</v>
+      </c>
+      <c r="D26">
+        <v>10</v>
+      </c>
+      <c r="E26">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F26">
+        <v>20000</v>
+      </c>
+      <c r="G26" t="s">
+        <v>63</v>
+      </c>
+      <c r="H26" t="s">
+        <v>89</v>
+      </c>
+      <c r="I26" t="s">
+        <v>76</v>
+      </c>
+      <c r="J26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" t="s">
+        <v>84</v>
+      </c>
+      <c r="D27">
+        <v>14</v>
+      </c>
+      <c r="E27">
+        <v>0.8</v>
+      </c>
+      <c r="F27">
+        <v>16000</v>
+      </c>
+      <c r="G27" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I27" t="s">
+        <v>75</v>
+      </c>
+      <c r="J27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" t="s">
+        <v>84</v>
+      </c>
+      <c r="D28">
+        <v>7</v>
+      </c>
+      <c r="E28">
+        <v>1.8</v>
+      </c>
+      <c r="F28">
+        <v>22000</v>
+      </c>
+      <c r="G28" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" t="s">
+        <v>73</v>
+      </c>
+      <c r="I28" t="s">
+        <v>62</v>
+      </c>
+      <c r="J28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29">
+        <v>9</v>
+      </c>
+      <c r="E29">
+        <v>1.3</v>
+      </c>
+      <c r="F29">
+        <v>21000</v>
+      </c>
+      <c r="G29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" t="s">
+        <v>98</v>
+      </c>
+      <c r="I29" t="s">
+        <v>97</v>
+      </c>
+      <c r="J29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>53</v>
+      </c>
+      <c r="C30" t="s">
+        <v>85</v>
+      </c>
+      <c r="D30">
+        <v>12</v>
+      </c>
+      <c r="E30">
+        <v>0.7</v>
+      </c>
+      <c r="F30">
+        <v>20000</v>
+      </c>
+      <c r="G30" t="s">
+        <v>69</v>
+      </c>
+      <c r="H30" t="s">
+        <v>96</v>
+      </c>
+      <c r="I30" t="s">
+        <v>70</v>
+      </c>
+      <c r="J30">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33">
+        <v>10</v>
+      </c>
+      <c r="E33">
+        <v>0.3</v>
+      </c>
+      <c r="F33">
+        <v>19000</v>
+      </c>
+      <c r="G33" t="s">
+        <v>79</v>
+      </c>
+      <c r="H33" t="s">
+        <v>99</v>
+      </c>
+      <c r="I33" t="s">
+        <v>62</v>
+      </c>
+      <c r="J33">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>81</v>
+      </c>
+      <c r="C34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34">
+        <v>15</v>
+      </c>
+      <c r="E34">
+        <v>0.5</v>
+      </c>
+      <c r="F34">
+        <v>19000</v>
+      </c>
+      <c r="G34" t="s">
+        <v>82</v>
+      </c>
+      <c r="H34" t="s">
+        <v>100</v>
+      </c>
+      <c r="I34" t="s">
+        <v>62</v>
+      </c>
+      <c r="J34">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="C35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35">
+        <v>8</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>18000</v>
+      </c>
+      <c r="G35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H35" t="s">
+        <v>102</v>
+      </c>
+      <c r="I35" t="s">
+        <v>101</v>
+      </c>
+      <c r="J35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38">
+        <v>11</v>
+      </c>
+      <c r="E38">
+        <v>0.9</v>
+      </c>
+      <c r="F38">
+        <v>22000</v>
+      </c>
+      <c r="G38" t="s">
+        <v>109</v>
+      </c>
+      <c r="H38" t="s">
+        <v>110</v>
+      </c>
+      <c r="I38" t="s">
+        <v>111</v>
+      </c>
+      <c r="J38" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" t="s">
+        <v>108</v>
+      </c>
+      <c r="D39">
+        <v>9</v>
+      </c>
+      <c r="E39">
+        <v>0.7</v>
+      </c>
+      <c r="F39">
+        <v>23000</v>
+      </c>
+      <c r="G39" t="s">
+        <v>109</v>
+      </c>
+      <c r="H39" t="s">
+        <v>112</v>
+      </c>
+      <c r="I39" t="s">
+        <v>111</v>
+      </c>
+      <c r="J39" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" t="s">
+        <v>84</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>0.5</v>
+      </c>
+      <c r="F40">
+        <v>20000</v>
+      </c>
+      <c r="G40" t="s">
+        <v>113</v>
+      </c>
+      <c r="H40" t="s">
+        <v>114</v>
+      </c>
+      <c r="I40" t="s">
+        <v>62</v>
+      </c>
+      <c r="J40" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" t="s">
+        <v>85</v>
+      </c>
+      <c r="D41">
+        <v>7</v>
+      </c>
+      <c r="E41">
+        <v>0.2</v>
+      </c>
+      <c r="F41">
+        <v>20000</v>
+      </c>
+      <c r="G41" t="s">
+        <v>116</v>
+      </c>
+      <c r="H41" t="s">
+        <v>117</v>
+      </c>
+      <c r="I41" t="s">
+        <v>62</v>
+      </c>
+      <c r="J41">
+        <v>20000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
@@ -858,10 +1918,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -886,10 +1946,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>